<commit_message>
Enforces angle brackets on Metadata URIs.
</commit_message>
<xml_diff>
--- a/src/test/resources/loaderfail5.xlsx
+++ b/src/test/resources/loaderfail5.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Sheet Name</t>
   </si>
@@ -75,15 +75,6 @@
   </si>
   <si>
     <t>@base</t>
-  </si>
-  <si>
-    <t>http://sales.data/purchases/2015</t>
-  </si>
-  <si>
-    <t>http://sales.data/purchases#</t>
-  </si>
-  <si>
-    <t>http://sales.data/schema#</t>
   </si>
   <si>
     <t>@prefix</t>
@@ -642,7 +633,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,62 +653,62 @@
         <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -741,7 +732,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>

</xml_diff>